<commit_message>
Updated version of data dictionary from Ken.
</commit_message>
<xml_diff>
--- a/labs/clinical-data-dictonary.xlsx
+++ b/labs/clinical-data-dictonary.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nrejack/code/hcv-target-sites/labs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/UFBuck72/TEMP/UF/target_2_0/research_missing_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{639058BB-06DD-6E48-888F-152C5C799F3E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="28340" tabRatio="500"/>
+    <workbookView xWindow="3600" yWindow="4320" windowWidth="25600" windowHeight="15740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataDictionaryforREDI" sheetId="1" r:id="rId1"/>
     <sheet name="modifiedREDCapDictionary" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -4107,7 +4108,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -4145,7 +4146,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4176,6 +4177,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -4201,7 +4208,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -4221,6 +4228,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4244,6 +4254,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -4570,16 +4583,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="4" max="4" width="38.33203125" customWidth="1"/>
     <col min="6" max="6" width="18.5" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" customWidth="1"/>
     <col min="8" max="8" width="23.5" customWidth="1"/>
@@ -6257,47 +6271,47 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" t="s">
+    <row r="40" spans="1:14" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="7" t="s">
         <v>1329</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="7" t="s">
         <v>717</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="7" t="s">
         <v>722</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="7" t="s">
         <v>444</v>
       </c>
-      <c r="G40" t="s">
-        <v>1301</v>
-      </c>
-      <c r="H40" t="s">
-        <v>1301</v>
-      </c>
-      <c r="I40" t="s">
-        <v>1301</v>
-      </c>
-      <c r="J40" t="s">
-        <v>1301</v>
-      </c>
-      <c r="K40" t="s">
-        <v>1301</v>
-      </c>
-      <c r="L40" t="s">
-        <v>1301</v>
-      </c>
-      <c r="M40" t="s">
-        <v>1301</v>
-      </c>
-      <c r="N40" t="s">
+      <c r="G40" s="7" t="s">
+        <v>1301</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>1301</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>1301</v>
+      </c>
+      <c r="J40" s="7" t="s">
+        <v>1301</v>
+      </c>
+      <c r="K40" s="7" t="s">
+        <v>1301</v>
+      </c>
+      <c r="L40" s="7" t="s">
+        <v>1301</v>
+      </c>
+      <c r="M40" s="7" t="s">
+        <v>1301</v>
+      </c>
+      <c r="N40" s="7" t="s">
         <v>1301</v>
       </c>
     </row>
@@ -6473,7 +6487,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AM464"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6775,7 +6789,7 @@
         <v>184100006</v>
       </c>
     </row>
-    <row r="7" spans="1:39" ht="91" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:39" ht="104" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -6812,7 +6826,7 @@
         <v>103579009</v>
       </c>
     </row>
-    <row r="8" spans="1:39" ht="39" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:39" ht="52" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -7353,7 +7367,7 @@
       <c r="Z23" s="4"/>
       <c r="AA23" s="4"/>
     </row>
-    <row r="24" spans="1:27" ht="78" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:27" ht="91" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>104</v>
       </c>
@@ -7387,7 +7401,7 @@
       <c r="Z24" s="4"/>
       <c r="AA24" s="4"/>
     </row>
-    <row r="25" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:27" ht="26" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>108</v>
       </c>
@@ -8667,7 +8681,7 @@
       <c r="Z65" s="4"/>
       <c r="AA65" s="4"/>
     </row>
-    <row r="66" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:27" ht="26" x14ac:dyDescent="0.15">
       <c r="A66" t="s">
         <v>206</v>
       </c>
@@ -9238,7 +9252,7 @@
       <c r="Z84" s="4"/>
       <c r="AA84" s="4"/>
     </row>
-    <row r="85" spans="1:27" ht="39" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:27" ht="52" x14ac:dyDescent="0.15">
       <c r="A85" t="s">
         <v>244</v>
       </c>
@@ -9520,7 +9534,7 @@
       <c r="Z93" s="4"/>
       <c r="AA93" s="4"/>
     </row>
-    <row r="94" spans="1:27" ht="409" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:27" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A94" t="s">
         <v>271</v>
       </c>
@@ -9734,7 +9748,7 @@
       <c r="Z100" s="4"/>
       <c r="AA100" s="4"/>
     </row>
-    <row r="101" spans="1:27" ht="409" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:27" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A101" t="s">
         <v>287</v>
       </c>
@@ -9799,7 +9813,7 @@
       <c r="Z102" s="4"/>
       <c r="AA102" s="4"/>
     </row>
-    <row r="103" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:27" ht="26" x14ac:dyDescent="0.15">
       <c r="A103" t="s">
         <v>295</v>
       </c>
@@ -9827,7 +9841,7 @@
       <c r="Z103" s="4"/>
       <c r="AA103" s="4"/>
     </row>
-    <row r="104" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:27" ht="26" x14ac:dyDescent="0.15">
       <c r="A104" t="s">
         <v>298</v>
       </c>
@@ -9855,7 +9869,7 @@
       <c r="Z104" s="4"/>
       <c r="AA104" s="4"/>
     </row>
-    <row r="105" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:27" ht="26" x14ac:dyDescent="0.15">
       <c r="A105" t="s">
         <v>300</v>
       </c>
@@ -9886,7 +9900,7 @@
       <c r="Z105" s="4"/>
       <c r="AA105" s="4"/>
     </row>
-    <row r="106" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:27" ht="26" x14ac:dyDescent="0.15">
       <c r="A106" t="s">
         <v>302</v>
       </c>
@@ -9920,7 +9934,7 @@
       <c r="Z106" s="4"/>
       <c r="AA106" s="4"/>
     </row>
-    <row r="107" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:27" ht="26" x14ac:dyDescent="0.15">
       <c r="A107" t="s">
         <v>305</v>
       </c>
@@ -9948,7 +9962,7 @@
       <c r="Z107" s="4"/>
       <c r="AA107" s="4"/>
     </row>
-    <row r="108" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:27" ht="26" x14ac:dyDescent="0.15">
       <c r="A108" t="s">
         <v>307</v>
       </c>
@@ -9976,7 +9990,7 @@
       <c r="Z108" s="4"/>
       <c r="AA108" s="4"/>
     </row>
-    <row r="109" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:27" ht="26" x14ac:dyDescent="0.15">
       <c r="A109" t="s">
         <v>309</v>
       </c>
@@ -10007,7 +10021,7 @@
       <c r="Z109" s="4"/>
       <c r="AA109" s="4"/>
     </row>
-    <row r="110" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:27" ht="26" x14ac:dyDescent="0.15">
       <c r="A110" t="s">
         <v>311</v>
       </c>
@@ -10044,7 +10058,7 @@
       <c r="Z110" s="4"/>
       <c r="AA110" s="4"/>
     </row>
-    <row r="111" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:27" ht="26" x14ac:dyDescent="0.15">
       <c r="A111" t="s">
         <v>314</v>
       </c>
@@ -10078,7 +10092,7 @@
       <c r="Z111" s="4"/>
       <c r="AA111" s="4"/>
     </row>
-    <row r="112" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:27" ht="26" x14ac:dyDescent="0.15">
       <c r="A112" t="s">
         <v>317</v>
       </c>
@@ -10146,7 +10160,7 @@
       <c r="Z113" s="4"/>
       <c r="AA113" s="4"/>
     </row>
-    <row r="114" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:27" ht="26" x14ac:dyDescent="0.15">
       <c r="A114" t="s">
         <v>324</v>
       </c>
@@ -10174,7 +10188,7 @@
       <c r="Z114" s="4"/>
       <c r="AA114" s="4"/>
     </row>
-    <row r="115" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:27" ht="26" x14ac:dyDescent="0.15">
       <c r="A115" t="s">
         <v>326</v>
       </c>
@@ -10202,7 +10216,7 @@
       <c r="Z115" s="4"/>
       <c r="AA115" s="4"/>
     </row>
-    <row r="116" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:27" ht="26" x14ac:dyDescent="0.15">
       <c r="A116" t="s">
         <v>328</v>
       </c>
@@ -10233,7 +10247,7 @@
       <c r="Z116" s="4"/>
       <c r="AA116" s="4"/>
     </row>
-    <row r="117" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:27" ht="26" x14ac:dyDescent="0.15">
       <c r="A117" t="s">
         <v>330</v>
       </c>
@@ -10295,7 +10309,7 @@
       <c r="Z118" s="4"/>
       <c r="AA118" s="4"/>
     </row>
-    <row r="119" spans="1:27" ht="39" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:27" ht="52" x14ac:dyDescent="0.15">
       <c r="A119" t="s">
         <v>336</v>
       </c>
@@ -10965,7 +10979,7 @@
       <c r="Z140" s="4"/>
       <c r="AA140" s="4"/>
     </row>
-    <row r="141" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:27" ht="26" x14ac:dyDescent="0.15">
       <c r="A141" t="s">
         <v>385</v>
       </c>
@@ -11064,7 +11078,7 @@
       <c r="Z143" s="4"/>
       <c r="AA143" s="4"/>
     </row>
-    <row r="144" spans="1:27" ht="39" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:27" ht="52" x14ac:dyDescent="0.15">
       <c r="A144" t="s">
         <v>394</v>
       </c>
@@ -15089,7 +15103,7 @@
       <c r="Z258" s="4"/>
       <c r="AA258" s="4"/>
     </row>
-    <row r="259" spans="1:27" ht="52" x14ac:dyDescent="0.15">
+    <row r="259" spans="1:27" ht="65" x14ac:dyDescent="0.15">
       <c r="A259" t="s">
         <v>735</v>
       </c>
@@ -15439,7 +15453,7 @@
       <c r="Z268" s="4"/>
       <c r="AA268" s="4"/>
     </row>
-    <row r="269" spans="1:27" ht="26" x14ac:dyDescent="0.15">
+    <row r="269" spans="1:27" ht="39" x14ac:dyDescent="0.15">
       <c r="A269" t="s">
         <v>768</v>
       </c>
@@ -15470,7 +15484,7 @@
       <c r="Z269" s="4"/>
       <c r="AA269" s="4"/>
     </row>
-    <row r="270" spans="1:27" ht="182" x14ac:dyDescent="0.15">
+    <row r="270" spans="1:27" ht="195" x14ac:dyDescent="0.15">
       <c r="A270" t="s">
         <v>771</v>
       </c>
@@ -16057,7 +16071,7 @@
       <c r="Z286" s="4"/>
       <c r="AA286" s="4"/>
     </row>
-    <row r="287" spans="1:27" ht="26" x14ac:dyDescent="0.15">
+    <row r="287" spans="1:27" ht="39" x14ac:dyDescent="0.15">
       <c r="A287" t="s">
         <v>821</v>
       </c>
@@ -16088,7 +16102,7 @@
       <c r="Z287" s="4"/>
       <c r="AA287" s="4"/>
     </row>
-    <row r="288" spans="1:27" ht="182" x14ac:dyDescent="0.15">
+    <row r="288" spans="1:27" ht="195" x14ac:dyDescent="0.15">
       <c r="A288" t="s">
         <v>824</v>
       </c>
@@ -16610,7 +16624,7 @@
       <c r="Z302" s="4"/>
       <c r="AA302" s="4"/>
     </row>
-    <row r="303" spans="1:27" ht="26" x14ac:dyDescent="0.15">
+    <row r="303" spans="1:27" ht="39" x14ac:dyDescent="0.15">
       <c r="A303" t="s">
         <v>867</v>
       </c>
@@ -16641,7 +16655,7 @@
       <c r="Z303" s="4"/>
       <c r="AA303" s="4"/>
     </row>
-    <row r="304" spans="1:27" ht="182" x14ac:dyDescent="0.15">
+    <row r="304" spans="1:27" ht="195" x14ac:dyDescent="0.15">
       <c r="A304" t="s">
         <v>870</v>
       </c>
@@ -17163,7 +17177,7 @@
       <c r="Z318" s="4"/>
       <c r="AA318" s="4"/>
     </row>
-    <row r="319" spans="1:27" ht="26" x14ac:dyDescent="0.15">
+    <row r="319" spans="1:27" ht="39" x14ac:dyDescent="0.15">
       <c r="A319" t="s">
         <v>911</v>
       </c>
@@ -17194,7 +17208,7 @@
       <c r="Z319" s="4"/>
       <c r="AA319" s="4"/>
     </row>
-    <row r="320" spans="1:27" ht="182" x14ac:dyDescent="0.15">
+    <row r="320" spans="1:27" ht="195" x14ac:dyDescent="0.15">
       <c r="A320" t="s">
         <v>914</v>
       </c>
@@ -17716,7 +17730,7 @@
       <c r="Z334" s="4"/>
       <c r="AA334" s="4"/>
     </row>
-    <row r="335" spans="1:27" ht="26" x14ac:dyDescent="0.15">
+    <row r="335" spans="1:27" ht="39" x14ac:dyDescent="0.15">
       <c r="A335" t="s">
         <v>956</v>
       </c>
@@ -17747,7 +17761,7 @@
       <c r="Z335" s="4"/>
       <c r="AA335" s="4"/>
     </row>
-    <row r="336" spans="1:27" ht="182" x14ac:dyDescent="0.15">
+    <row r="336" spans="1:27" ht="195" x14ac:dyDescent="0.15">
       <c r="A336" t="s">
         <v>959</v>
       </c>
@@ -18269,7 +18283,7 @@
       <c r="Z350" s="4"/>
       <c r="AA350" s="4"/>
     </row>
-    <row r="351" spans="1:27" ht="26" x14ac:dyDescent="0.15">
+    <row r="351" spans="1:27" ht="39" x14ac:dyDescent="0.15">
       <c r="A351" t="s">
         <v>1000</v>
       </c>
@@ -18300,7 +18314,7 @@
       <c r="Z351" s="4"/>
       <c r="AA351" s="4"/>
     </row>
-    <row r="352" spans="1:27" ht="182" x14ac:dyDescent="0.15">
+    <row r="352" spans="1:27" ht="195" x14ac:dyDescent="0.15">
       <c r="A352" t="s">
         <v>1003</v>
       </c>
@@ -18578,7 +18592,7 @@
       <c r="Z359" s="4"/>
       <c r="AA359" s="4"/>
     </row>
-    <row r="360" spans="1:27" ht="182" x14ac:dyDescent="0.15">
+    <row r="360" spans="1:27" ht="195" x14ac:dyDescent="0.15">
       <c r="A360" t="s">
         <v>1027</v>
       </c>
@@ -18649,7 +18663,7 @@
       <c r="Z361" s="4"/>
       <c r="AA361" s="4"/>
     </row>
-    <row r="362" spans="1:27" ht="286" x14ac:dyDescent="0.15">
+    <row r="362" spans="1:27" ht="312" x14ac:dyDescent="0.15">
       <c r="A362" t="s">
         <v>1033</v>
       </c>
@@ -19001,7 +19015,7 @@
       <c r="Z371" s="4"/>
       <c r="AA371" s="4"/>
     </row>
-    <row r="372" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="372" spans="1:27" ht="26" x14ac:dyDescent="0.15">
       <c r="A372" t="s">
         <v>1062</v>
       </c>
@@ -19171,7 +19185,7 @@
       <c r="Z376" s="4"/>
       <c r="AA376" s="4"/>
     </row>
-    <row r="377" spans="1:27" ht="39" x14ac:dyDescent="0.15">
+    <row r="377" spans="1:27" ht="52" x14ac:dyDescent="0.15">
       <c r="A377" t="s">
         <v>1076</v>
       </c>
@@ -19239,7 +19253,7 @@
       <c r="Z378" s="4"/>
       <c r="AA378" s="4"/>
     </row>
-    <row r="379" spans="1:27" ht="104" x14ac:dyDescent="0.15">
+    <row r="379" spans="1:27" ht="117" x14ac:dyDescent="0.15">
       <c r="A379" t="s">
         <v>1080</v>
       </c>
@@ -19452,7 +19466,7 @@
       <c r="Z384" s="4"/>
       <c r="AA384" s="4"/>
     </row>
-    <row r="385" spans="1:27" ht="182" x14ac:dyDescent="0.15">
+    <row r="385" spans="1:27" ht="195" x14ac:dyDescent="0.15">
       <c r="A385" t="s">
         <v>1100</v>
       </c>
@@ -19984,7 +19998,7 @@
       <c r="Z400" s="4"/>
       <c r="AA400" s="4"/>
     </row>
-    <row r="401" spans="1:27" ht="182" x14ac:dyDescent="0.15">
+    <row r="401" spans="1:27" ht="195" x14ac:dyDescent="0.15">
       <c r="A401" t="s">
         <v>1140</v>
       </c>
@@ -20390,7 +20404,7 @@
       <c r="Z413" s="4"/>
       <c r="AA413" s="4"/>
     </row>
-    <row r="414" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="414" spans="1:27" ht="26" x14ac:dyDescent="0.15">
       <c r="A414" t="s">
         <v>1174</v>
       </c>

</xml_diff>